<commit_message>
working on css style
</commit_message>
<xml_diff>
--- a/my-app/src/data/questionnaries.xlsx
+++ b/my-app/src/data/questionnaries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="159">
   <si>
     <t>i11</t>
   </si>
@@ -68,18 +68,9 @@
     <t>i25</t>
   </si>
   <si>
-    <t>i31</t>
-  </si>
-  <si>
-    <t>i32</t>
-  </si>
-  <si>
     <t>i33</t>
   </si>
   <si>
-    <t>i41</t>
-  </si>
-  <si>
     <t>i42</t>
   </si>
   <si>
@@ -92,9 +83,6 @@
     <t>question</t>
   </si>
   <si>
-    <t>idicateur</t>
-  </si>
-  <si>
     <t>option1</t>
   </si>
   <si>
@@ -143,18 +131,12 @@
     <t>Formation universitaire, Haute école</t>
   </si>
   <si>
-    <t>Langue maternelle</t>
-  </si>
-  <si>
     <t>Français</t>
   </si>
   <si>
     <t>Autre</t>
   </si>
   <si>
-    <t>Votre origine</t>
-  </si>
-  <si>
     <t>Lausanne et région</t>
   </si>
   <si>
@@ -170,9 +152,6 @@
     <t>Vous utilisez des smartphones/tablettes tactile</t>
   </si>
   <si>
-    <t>titre</t>
-  </si>
-  <si>
     <t>Avant de commencer, nous aimerions en savoir un peu plus sur…</t>
   </si>
   <si>
@@ -191,18 +170,12 @@
     <t>slider</t>
   </si>
   <si>
-    <t>Sur une échelle de 1 à 5, évaluez votre niveau dans les domaines suivants (1 faible, 5 élevé)</t>
-  </si>
-  <si>
     <t>Lecture de carte</t>
   </si>
   <si>
     <t>Sens de l'orientation</t>
   </si>
   <si>
-    <t>Sur une échelle de 1 à 5, évaluez votre intérêt dans ces différents domaines (1 faible, 5 élevé)</t>
-  </si>
-  <si>
     <t>Géomorphologie</t>
   </si>
   <si>
@@ -327,6 +300,210 @@
   </si>
   <si>
     <t>Je n'ai pas d'attente patriculières</t>
+  </si>
+  <si>
+    <t>i311</t>
+  </si>
+  <si>
+    <t>i312</t>
+  </si>
+  <si>
+    <t>i322</t>
+  </si>
+  <si>
+    <t>i323</t>
+  </si>
+  <si>
+    <t>i325</t>
+  </si>
+  <si>
+    <t>i324</t>
+  </si>
+  <si>
+    <t>La Louve et Le Flon</t>
+  </si>
+  <si>
+    <t>La Louve et La Venoge</t>
+  </si>
+  <si>
+    <t>indicator</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>series</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En géomorphologie, lequel de ces termes désigne une forme sédimentaire d'origine glaciaire? </t>
+  </si>
+  <si>
+    <t>Un éboulis</t>
+  </si>
+  <si>
+    <t>Une gorge</t>
+  </si>
+  <si>
+    <t>Une moraine</t>
+  </si>
+  <si>
+    <t>Un bassin versant</t>
+  </si>
+  <si>
+    <t>Le relief Lausannois a notamment été dessiné par deux rivières. Il s'agit de :</t>
+  </si>
+  <si>
+    <t>La Venoge et Le Flon</t>
+  </si>
+  <si>
+    <t>Connaissez-vous la ville de Lausanne?</t>
+  </si>
+  <si>
+    <t>Le Flon et La Sorge</t>
+  </si>
+  <si>
+    <t>La Cité</t>
+  </si>
+  <si>
+    <t>La Riponne</t>
+  </si>
+  <si>
+    <t>conclusion</t>
+  </si>
+  <si>
+    <t>introduction</t>
+  </si>
+  <si>
+    <t>L'hydrogaphie</t>
+  </si>
+  <si>
+    <t>Le climat</t>
+  </si>
+  <si>
+    <t>A Lausanne, lequel de ces quartiers n'a pas connu de projet d'aménagement d'envergure durant les deux derniers siècles?</t>
+  </si>
+  <si>
+    <t>i313</t>
+  </si>
+  <si>
+    <t>i314</t>
+  </si>
+  <si>
+    <t>i315</t>
+  </si>
+  <si>
+    <t>i321</t>
+  </si>
+  <si>
+    <t>Dans l'histoire de Lausanne, lequel de ces éléments n'a pas eu d'impact sur la structure de la ville d'aujourd'hui?</t>
+  </si>
+  <si>
+    <t>Les grands projets d'aménagement urbains</t>
+  </si>
+  <si>
+    <t>Aucun; tous ces éléments ont joué un rôle dans la structure de la ville telle que nous la connaissons aujourd'hui</t>
+  </si>
+  <si>
+    <t>La topographie</t>
+  </si>
+  <si>
+    <t>La Louve et La Sorge</t>
+  </si>
+  <si>
+    <t>Dans l'histoire de Lausanne, lequel de ces éléments n'a  pas impacté la structure de la ville d'aujourd'hui?</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>lausanne knowledge</t>
+  </si>
+  <si>
+    <t>Vous êtes originaire de…</t>
+  </si>
+  <si>
+    <t>Le Géoguide fonctionne sur votre téléphone, c'est super! Mais vous…</t>
+  </si>
+  <si>
+    <t>user habits</t>
+  </si>
+  <si>
+    <t>Vous êtes sur le bon chemin!</t>
+  </si>
+  <si>
+    <t>user abilities</t>
+  </si>
+  <si>
+    <t>Sur une échelle de 1 à 5, évaluez votre niveau dans les domaines suivants (1 =aible, 5=élevé)</t>
+  </si>
+  <si>
+    <t>Le Géoguide contient beaucoup d'informations sur des domaines très spécifiques… Et vous, qu'est-ce qui vous intéresse?</t>
+  </si>
+  <si>
+    <t>Sur une échelle de 1 à 5, évaluez votre intérêt dans ces différents domaines (1 =aible, 5=élevé)</t>
+  </si>
+  <si>
+    <t>Nous sommes enfin arrivés, mais nous avons encore quelques petites questions!</t>
+  </si>
+  <si>
+    <t>Je n'ai pas fait les quiz!</t>
+  </si>
+  <si>
+    <t>Commençons par un petit test de connaissance</t>
+  </si>
+  <si>
+    <t>Revenons aux questions de départ!</t>
+  </si>
+  <si>
+    <t>i411</t>
+  </si>
+  <si>
+    <t>i41img1.jpg</t>
+  </si>
+  <si>
+    <t>i412</t>
+  </si>
+  <si>
+    <t>Grancy</t>
+  </si>
+  <si>
+    <t>i41img2.jpg</t>
+  </si>
+  <si>
+    <t>i413</t>
+  </si>
+  <si>
+    <t>Parmi ces grans édifices lausannois, lequel n'apparaît pas sur cette photo?</t>
+  </si>
+  <si>
+    <t>Le Palais de Rhumine</t>
+  </si>
+  <si>
+    <t>La Cathédrale</t>
+  </si>
+  <si>
+    <t>La Tour Bel-Air</t>
+  </si>
+  <si>
+    <t>L'Eglise St-Laurent</t>
+  </si>
+  <si>
+    <t>i41img3.jpg</t>
+  </si>
+  <si>
+    <t>Pourriez-vous nous en dire plus sur vos loisirs?</t>
+  </si>
+  <si>
+    <t>user preferences</t>
+  </si>
+  <si>
+    <t>Nous allons bientôt partir à la re-découverte de Lausanne</t>
+  </si>
+  <si>
+    <t>Votre langue maternelle</t>
   </si>
 </sst>
 </file>
@@ -362,10 +539,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,496 +824,896 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="9" width="33.33203125" customWidth="1"/>
+    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="31" style="2" customWidth="1"/>
+    <col min="6" max="10" width="33.33203125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>158</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>63</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>73</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>72</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>79</v>
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>88</v>
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>99</v>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>